<commit_message>
website: arabic style & forms & search edit
</commit_message>
<xml_diff>
--- a/public/excel/standard.xlsx
+++ b/public/excel/standard.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Reham\Desktop\bs-center\public\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24F2853E-64B4-4BF7-A1C0-CD758CD4ED96}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C958BA31-A460-41EB-AC56-ABE8EF4CCFE3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="25">
   <si>
     <t>title</t>
   </si>
@@ -49,9 +49,6 @@
   </si>
   <si>
     <t>Reciprocating Compressor Maintenance and troubleshooting</t>
-  </si>
-  <si>
-    <t>5 Days</t>
   </si>
   <si>
     <t>Mechanical, Electrical, Telecom and Power engineering</t>
@@ -472,7 +469,7 @@
   <dimension ref="A1:H8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I3" sqref="I3"/>
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -504,24 +501,24 @@
         <v>6</v>
       </c>
       <c r="H1" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>7</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="2">
+        <v>5</v>
+      </c>
+      <c r="C2" t="s">
         <v>8</v>
-      </c>
-      <c r="C2" t="s">
-        <v>9</v>
       </c>
       <c r="D2" s="2">
         <v>4300</v>
       </c>
       <c r="E2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F2" s="3">
         <v>45292</v>
@@ -530,24 +527,24 @@
         <v>45296</v>
       </c>
       <c r="H2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>12</v>
-      </c>
-      <c r="B3" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3" s="2">
+        <v>5</v>
+      </c>
+      <c r="C3" t="s">
         <v>8</v>
-      </c>
-      <c r="C3" t="s">
-        <v>9</v>
       </c>
       <c r="D3" s="2">
         <v>6100</v>
       </c>
       <c r="E3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F3" s="3">
         <v>45299</v>
@@ -556,24 +553,24 @@
         <v>45303</v>
       </c>
       <c r="H3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>14</v>
-      </c>
-      <c r="B4" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B4" s="2">
+        <v>3</v>
+      </c>
+      <c r="C4" t="s">
         <v>8</v>
-      </c>
-      <c r="C4" t="s">
-        <v>9</v>
       </c>
       <c r="D4" s="2">
         <v>4300</v>
       </c>
       <c r="E4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F4" s="3">
         <v>45306</v>
@@ -582,24 +579,24 @@
         <v>45310</v>
       </c>
       <c r="H4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
+        <v>15</v>
+      </c>
+      <c r="B5" s="2">
+        <v>5</v>
+      </c>
+      <c r="C5" t="s">
         <v>16</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="C5" t="s">
-        <v>17</v>
       </c>
       <c r="D5" s="2">
         <v>4300</v>
       </c>
       <c r="E5" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F5" s="3">
         <v>45313</v>
@@ -608,24 +605,24 @@
         <v>45317</v>
       </c>
       <c r="H5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>19</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>8</v>
+        <v>18</v>
+      </c>
+      <c r="B6" s="2">
+        <v>1</v>
       </c>
       <c r="C6" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D6" s="2">
         <v>4300</v>
       </c>
       <c r="E6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F6" s="3">
         <v>45320</v>
@@ -634,24 +631,24 @@
         <v>45324</v>
       </c>
       <c r="H6" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>21</v>
-      </c>
-      <c r="B7" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B7" s="2">
+        <v>2</v>
+      </c>
+      <c r="C7" t="s">
         <v>8</v>
-      </c>
-      <c r="C7" t="s">
-        <v>9</v>
       </c>
       <c r="D7" s="2">
         <v>6100</v>
       </c>
       <c r="E7" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F7" s="3">
         <v>45327</v>
@@ -660,24 +657,24 @@
         <v>45331</v>
       </c>
       <c r="H7" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>23</v>
-      </c>
-      <c r="B8" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B8" s="2">
+        <v>9</v>
+      </c>
+      <c r="C8" t="s">
         <v>8</v>
-      </c>
-      <c r="C8" t="s">
-        <v>9</v>
       </c>
       <c r="D8" s="2">
         <v>6100</v>
       </c>
       <c r="E8" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F8" s="3">
         <v>45334</v>
@@ -686,7 +683,7 @@
         <v>45338</v>
       </c>
       <c r="H8" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>